<commit_message>
Commentaires dans le code
</commit_message>
<xml_diff>
--- a/Plan de tests.xlsx
+++ b/Plan de tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\IdeaProjects\DAMMNicolas_5_16112020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89654159-3E43-4411-8A58-E30BF78C8666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BD938-5782-449E-8C0A-98E5333F53CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,21 +43,12 @@
     <t>basket.service.js</t>
   </si>
   <si>
-    <t>11 à 13</t>
-  </si>
-  <si>
     <t>saveBasket</t>
   </si>
   <si>
-    <t>Le méthode doit transformer en json l'objet "basket" et l'enregistrer dans le localStorage</t>
-  </si>
-  <si>
     <t>Appeler la méthode "saveBasket" de la class "Basket"</t>
   </si>
   <si>
-    <t>14 à 17</t>
-  </si>
-  <si>
     <t>cancelBasket</t>
   </si>
   <si>
@@ -67,21 +58,9 @@
     <t>Le panier pourrait ne pas se vider</t>
   </si>
   <si>
-    <t>18 à 36</t>
-  </si>
-  <si>
     <t>setProduct</t>
   </si>
   <si>
-    <t>La méthode doit vider le panier en réinitialisant l'objet "basket" à partir du model "MasketModel"</t>
-  </si>
-  <si>
-    <t>La methode doit ajouter un produit au panier si il n'éxiste pas à partir du model ProductModel ou si le produit existe déjà augmenter son nombre, ajouter une customization et aditionner le prix total</t>
-  </si>
-  <si>
-    <t>37 à 55</t>
-  </si>
-  <si>
     <t>deleteProduct</t>
   </si>
   <si>
@@ -100,9 +79,6 @@
     <t>L'objet du produit pourrait ne pas se supprimer ou ne pas réduire son nombre total et son prix dans le cas ou il est ajouté plusieurs fois</t>
   </si>
   <si>
-    <t>56 à 58</t>
-  </si>
-  <si>
     <t>countTotalArticles</t>
   </si>
   <si>
@@ -112,9 +88,6 @@
     <t>Le nombre de produits dans le panier pourrait ne pas être le bon, ou ne pas s'afficher du tout.</t>
   </si>
   <si>
-    <t>59 à 65</t>
-  </si>
-  <si>
     <t>getAllProducts</t>
   </si>
   <si>
@@ -124,18 +97,12 @@
     <t>L'objet retourné pourrait ne pas contenir les bonnes données</t>
   </si>
   <si>
-    <t>66 à 79</t>
-  </si>
-  <si>
     <t>getAllIdByShop</t>
   </si>
   <si>
     <t>Appeler la méthode "getAllIdByShop" de la class "Basket"</t>
   </si>
   <si>
-    <t>80 à 92</t>
-  </si>
-  <si>
     <t>getLastPicturesByShop</t>
   </si>
   <si>
@@ -148,9 +115,6 @@
     <t xml:space="preserve">Le nombre d'images retournés pourrait être incomplet </t>
   </si>
   <si>
-    <t>93 à 95</t>
-  </si>
-  <si>
     <t>getTotalPrice</t>
   </si>
   <si>
@@ -160,21 +124,12 @@
     <t xml:space="preserve">Le prix total pourrait être erroné </t>
   </si>
   <si>
-    <t>96 à 98</t>
-  </si>
-  <si>
     <t>getTotalPriceByProduct</t>
   </si>
   <si>
-    <t>99 à 105</t>
-  </si>
-  <si>
     <t>getTotalPriceByShop</t>
   </si>
   <si>
-    <t>106 à 112</t>
-  </si>
-  <si>
     <t>getTotalArticlesByShop</t>
   </si>
   <si>
@@ -190,9 +145,6 @@
     <t>Le nombre total de produits pourrait être arroné</t>
   </si>
   <si>
-    <t>113 à 127</t>
-  </si>
-  <si>
     <t>verifForm</t>
   </si>
   <si>
@@ -205,9 +157,6 @@
     <t>confirmation.service.js</t>
   </si>
   <si>
-    <t>17 à 19</t>
-  </si>
-  <si>
     <t>saveConfirmation</t>
   </si>
   <si>
@@ -247,9 +196,6 @@
     <t>La valeur enregistrée pourrait être incorrecte</t>
   </si>
   <si>
-    <t>20 à 26</t>
-  </si>
-  <si>
     <t>orderCancel</t>
   </si>
   <si>
@@ -262,9 +208,6 @@
     <t>Les données de confirmation et du panier pourraient ne pas s'éffacer et le status de confirmation rester a "true"</t>
   </si>
   <si>
-    <t>27 à 33</t>
-  </si>
-  <si>
     <t>setConfirmation</t>
   </si>
   <si>
@@ -280,15 +223,9 @@
     <t>render.service.js</t>
   </si>
   <si>
-    <t>3 à 7</t>
-  </si>
-  <si>
     <t>Render</t>
   </si>
   <si>
-    <t>La function doit utiliser un id html pour y ajouter des données MustacheJS à l'intérieur</t>
-  </si>
-  <si>
     <t>Appeler la function "Render" avec les paramètres suivants: "id" et "data"</t>
   </si>
   <si>
@@ -298,19 +235,82 @@
     <t>route.service.js</t>
   </si>
   <si>
-    <t>1 à 13</t>
-  </si>
-  <si>
     <t>Route</t>
   </si>
   <si>
-    <t>La function doit récupérer le fichier de la template MustacheJS correspondant à la route via fetch et exécuter le controller associé</t>
-  </si>
-  <si>
     <t>Appeler la function "Route" avec les paramètres suivants: "route" et "controller"</t>
   </si>
   <si>
     <t xml:space="preserve">La template ou le controller pourrait ne pas se charger correctement </t>
+  </si>
+  <si>
+    <t>La methode doit ajouter un produit au panier si il n'existe pas à partir du model ProductModel ou si le produit existe déjà augmenter son nombre, ajouter une customization et additionner le prix total</t>
+  </si>
+  <si>
+    <t>La méthode doit vider le panier en réinitialisant l'objet "basket" à partir du model "BasketModel"</t>
+  </si>
+  <si>
+    <t>La méthode doit transformer en json l'objet "basket" et l'enregistrer dans le localStorage</t>
+  </si>
+  <si>
+    <t>La fonction doit utiliser un id html pour y ajouter des données MustacheJS à l'intérieur</t>
+  </si>
+  <si>
+    <t>La fonction doit récupérer le fichier de la template MustacheJS correspondant à la route via fetch et exécuter le controller associé</t>
+  </si>
+  <si>
+    <t>25 à 28</t>
+  </si>
+  <si>
+    <t>33 à 36</t>
+  </si>
+  <si>
+    <t>47 à 65</t>
+  </si>
+  <si>
+    <t>77 à 96</t>
+  </si>
+  <si>
+    <t>101 à 103</t>
+  </si>
+  <si>
+    <t>110 à 116</t>
+  </si>
+  <si>
+    <t>124 à 137</t>
+  </si>
+  <si>
+    <t>146 à 148</t>
+  </si>
+  <si>
+    <t>165 à 167</t>
+  </si>
+  <si>
+    <t>176 à 178</t>
+  </si>
+  <si>
+    <t>186 à 192</t>
+  </si>
+  <si>
+    <t>200 à 206</t>
+  </si>
+  <si>
+    <t>216 à 230</t>
+  </si>
+  <si>
+    <t>31 à 34</t>
+  </si>
+  <si>
+    <t>39 à 45</t>
+  </si>
+  <si>
+    <t>57 à 63</t>
+  </si>
+  <si>
+    <t>70 à 73</t>
+  </si>
+  <si>
+    <t>9 à 21</t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,19 +694,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -714,19 +714,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -734,19 +734,19 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -754,19 +754,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -774,19 +774,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -794,19 +794,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -814,19 +814,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -834,19 +834,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -854,19 +854,19 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -874,19 +874,19 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -894,19 +894,19 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -914,19 +914,19 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -934,119 +934,119 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="41" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>78</v>
-      </c>
       <c r="F17" s="10" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>